<commit_message>
Set exercises Q1 - updated graphs axis, Q1C valgrind analysis
</commit_message>
<xml_diff>
--- a/Set Exercises/data.xlsx
+++ b/Set Exercises/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\datgu\Documents\Code\parallel-computing\Set Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89FACEB-C09C-4FA2-8E30-5BC81E299547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AFD3EE-DD23-45FE-B1F1-6B545C7597CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4848" yWindow="828" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>N</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>4096*32</t>
+  </si>
+  <si>
+    <t>D1 misses</t>
+  </si>
+  <si>
+    <t>D refs</t>
+  </si>
+  <si>
+    <t>33% miss rate</t>
   </si>
 </sst>
 </file>
@@ -92,10 +101,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,7 +158,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>a. gigaFLOPS</a:t>
+              <a:t>q1a.c GFLOPS</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
@@ -501,7 +511,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>gigaFLOPS</a:t>
+                  <a:t>GFLOPS</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -659,15 +669,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>b.</a:t>
+              <a:t>q1b.</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
+              <a:t>c G</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>gigaFLOPS vs N</a:t>
+              <a:t>FLOPS vs N</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1035,7 +1045,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>gigaFLOPS</a:t>
+                  <a:t>GFLOPS</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2596,15 +2606,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2617,8 +2627,17 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2631,8 +2650,14 @@
       <c r="E2" s="2">
         <v>2.6</v>
       </c>
+      <c r="H2" s="3">
+        <v>2123067</v>
+      </c>
+      <c r="J2" s="3">
+        <v>6381601</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2645,8 +2670,10 @@
       <c r="E3" s="2">
         <v>2.5</v>
       </c>
+      <c r="H3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2660,7 +2687,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2674,7 +2701,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2688,7 +2715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D7" s="1">
         <v>8192</v>
       </c>
@@ -2696,7 +2723,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="D8" s="1">
         <v>16384</v>

</xml_diff>